<commit_message>
Update BlackJack -> Klassen-Auslagerung vorbereitet, Hit und Stand gefixt, buttonHelp und buttonZurueck hinzugefügt
Signed-off-by: albionspahija <32865170+albionspahija@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitplanungBlackJack.xlsx
+++ b/Dokumentation/ZeitplanungBlackJack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87B33BE-8B4E-4A7B-A709-1502C13C40E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21E8011-3573-4086-97BF-CCDB012CEDFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,12 +218,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AWR45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,21 +577,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1292" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:1292" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="4" spans="1:1292" x14ac:dyDescent="0.3">
       <c r="C4" s="4"/>
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="8"/>
       <c r="G4" t="s">
         <v>19</v>
       </c>
@@ -657,16 +657,16 @@
         <v>25</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="L7" s="8"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:1292" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
-      <c r="L8" s="8"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="C9" s="2"/>
-      <c r="L9" s="8"/>
+      <c r="L9" s="7"/>
       <c r="T9"/>
       <c r="U9"/>
       <c r="V9"/>
@@ -1947,7 +1947,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="L10" s="8"/>
+      <c r="L10" s="7"/>
       <c r="T10"/>
       <c r="U10"/>
       <c r="V10"/>
@@ -3225,7 +3225,7 @@
     <row r="11" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="D11" s="2"/>
-      <c r="L11" s="8"/>
+      <c r="L11" s="7"/>
       <c r="T11"/>
       <c r="U11"/>
       <c r="V11"/>
@@ -4502,7 +4502,7 @@
     </row>
     <row r="12" spans="1:1292" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
-      <c r="L12" s="8"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:1292" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -4511,13 +4511,14 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
-      <c r="L13" s="8"/>
+      <c r="H13" s="5"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="L14" s="8"/>
+      <c r="L14" s="7"/>
       <c r="T14"/>
       <c r="U14"/>
       <c r="V14"/>
@@ -5796,7 +5797,7 @@
       <c r="A15"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="L15" s="8"/>
+      <c r="L15" s="7"/>
       <c r="T15"/>
       <c r="U15"/>
       <c r="V15"/>
@@ -7071,13 +7072,13 @@
       <c r="AWQ15"/>
       <c r="AWR15"/>
     </row>
-    <row r="16" spans="1:1292" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1292" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="L16" s="8"/>
+      <c r="H16" s="4"/>
+      <c r="L16" s="7"/>
       <c r="T16"/>
       <c r="U16"/>
       <c r="V16"/>
@@ -8355,7 +8356,7 @@
     <row r="17" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="G17" s="2"/>
-      <c r="L17" s="8"/>
+      <c r="L17" s="7"/>
       <c r="T17"/>
       <c r="U17"/>
       <c r="V17"/>
@@ -9633,7 +9634,7 @@
     <row r="18" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="G18" s="2"/>
-      <c r="L18" s="8"/>
+      <c r="L18" s="7"/>
       <c r="T18"/>
       <c r="U18"/>
       <c r="V18"/>
@@ -10912,13 +10913,12 @@
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="5"/>
       <c r="H19" s="4"/>
-      <c r="L19" s="8"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
-      <c r="L20" s="8"/>
+      <c r="L20" s="7"/>
       <c r="T20"/>
       <c r="U20"/>
       <c r="V20"/>
@@ -12195,7 +12195,7 @@
     </row>
     <row r="21" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
-      <c r="L21" s="8"/>
+      <c r="L21" s="7"/>
       <c r="T21"/>
       <c r="U21"/>
       <c r="V21"/>
@@ -13477,7 +13477,7 @@
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="L22" s="8"/>
+      <c r="L22" s="7"/>
       <c r="T22"/>
       <c r="U22"/>
       <c r="V22"/>
@@ -14754,7 +14754,7 @@
     </row>
     <row r="23" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
-      <c r="L23" s="8"/>
+      <c r="L23" s="7"/>
       <c r="T23"/>
       <c r="U23"/>
       <c r="V23"/>
@@ -16031,7 +16031,7 @@
     </row>
     <row r="24" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
-      <c r="L24" s="8"/>
+      <c r="L24" s="7"/>
       <c r="T24"/>
       <c r="U24"/>
       <c r="V24"/>
@@ -17307,11 +17307,11 @@
       <c r="AWR24"/>
     </row>
     <row r="25" spans="1:1292" x14ac:dyDescent="0.3">
-      <c r="L25" s="8"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26"/>
-      <c r="L26" s="8"/>
+      <c r="L26" s="7"/>
       <c r="T26"/>
       <c r="U26"/>
       <c r="V26"/>
@@ -18588,7 +18588,7 @@
     </row>
     <row r="27" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
-      <c r="L27" s="8"/>
+      <c r="L27" s="7"/>
       <c r="T27"/>
       <c r="U27"/>
       <c r="V27"/>
@@ -19865,7 +19865,7 @@
     </row>
     <row r="28" spans="1:1292" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28"/>
-      <c r="L28" s="8"/>
+      <c r="L28" s="7"/>
       <c r="T28"/>
       <c r="U28"/>
       <c r="V28"/>
@@ -21142,7 +21142,7 @@
     </row>
     <row r="29" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
-      <c r="L29" s="8"/>
+      <c r="L29" s="7"/>
       <c r="T29"/>
       <c r="U29"/>
       <c r="V29"/>
@@ -22419,7 +22419,7 @@
     </row>
     <row r="30" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30"/>
-      <c r="L30" s="8"/>
+      <c r="L30" s="7"/>
       <c r="T30"/>
       <c r="U30"/>
       <c r="V30"/>
@@ -23695,11 +23695,11 @@
       <c r="AWR30"/>
     </row>
     <row r="31" spans="1:1292" x14ac:dyDescent="0.3">
-      <c r="L31" s="8"/>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32"/>
-      <c r="L32" s="8"/>
+      <c r="L32" s="7"/>
       <c r="T32"/>
       <c r="U32"/>
       <c r="V32"/>
@@ -24976,7 +24976,7 @@
     </row>
     <row r="33" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33"/>
-      <c r="L33" s="8"/>
+      <c r="L33" s="7"/>
       <c r="T33"/>
       <c r="U33"/>
       <c r="V33"/>
@@ -26253,7 +26253,7 @@
     </row>
     <row r="34" spans="1:1292" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34"/>
-      <c r="L34" s="8"/>
+      <c r="L34" s="7"/>
       <c r="T34"/>
       <c r="U34"/>
       <c r="V34"/>
@@ -27530,7 +27530,7 @@
     </row>
     <row r="35" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35"/>
-      <c r="L35" s="8"/>
+      <c r="L35" s="7"/>
       <c r="T35"/>
       <c r="U35"/>
       <c r="V35"/>
@@ -28807,7 +28807,7 @@
     </row>
     <row r="36" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36"/>
-      <c r="L36" s="8"/>
+      <c r="L36" s="7"/>
       <c r="T36"/>
       <c r="U36"/>
       <c r="V36"/>
@@ -30083,11 +30083,11 @@
       <c r="AWR36"/>
     </row>
     <row r="37" spans="1:1292" x14ac:dyDescent="0.3">
-      <c r="L37" s="8"/>
+      <c r="L37" s="7"/>
     </row>
     <row r="38" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38"/>
-      <c r="L38" s="8"/>
+      <c r="L38" s="7"/>
       <c r="T38"/>
       <c r="U38"/>
       <c r="V38"/>
@@ -31364,7 +31364,7 @@
     </row>
     <row r="39" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39"/>
-      <c r="L39" s="8"/>
+      <c r="L39" s="7"/>
       <c r="T39"/>
       <c r="U39"/>
       <c r="V39"/>
@@ -32641,7 +32641,7 @@
     </row>
     <row r="40" spans="1:1292" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40"/>
-      <c r="L40" s="8"/>
+      <c r="L40" s="7"/>
       <c r="T40"/>
       <c r="U40"/>
       <c r="V40"/>
@@ -33918,7 +33918,7 @@
     </row>
     <row r="41" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41"/>
-      <c r="L41" s="8"/>
+      <c r="L41" s="7"/>
       <c r="T41"/>
       <c r="U41"/>
       <c r="V41"/>
@@ -35195,7 +35195,7 @@
     </row>
     <row r="42" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42"/>
-      <c r="L42" s="8"/>
+      <c r="L42" s="7"/>
       <c r="T42"/>
       <c r="U42"/>
       <c r="V42"/>
@@ -36471,11 +36471,11 @@
       <c r="AWR42"/>
     </row>
     <row r="43" spans="1:1292" x14ac:dyDescent="0.3">
-      <c r="L43" s="8"/>
+      <c r="L43" s="7"/>
     </row>
     <row r="44" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44"/>
-      <c r="L44" s="8"/>
+      <c r="L44" s="7"/>
       <c r="T44"/>
       <c r="U44"/>
       <c r="V44"/>
@@ -37752,7 +37752,7 @@
     </row>
     <row r="45" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45"/>
-      <c r="L45" s="8"/>
+      <c r="L45" s="7"/>
       <c r="T45"/>
       <c r="U45"/>
       <c r="V45"/>

</xml_diff>

<commit_message>
Codefix BlackJack, Update Karten BlackJack
Signed-off-by: albionspahija <32865170+albionspahija@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitplanungBlackJack.xlsx
+++ b/Dokumentation/ZeitplanungBlackJack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21E8011-3573-4086-97BF-CCDB012CEDFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0599FEB5-A54A-41F2-ACD7-93B034E3E6BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +138,13 @@
       <b/>
       <sz val="28"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,7 +218,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1"/>
@@ -224,6 +231,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -243,8 +251,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3F3F"/>
       <color rgb="FF5BD171"/>
-      <color rgb="FFFF3F3F"/>
     </mruColors>
   </colors>
   <extLst>
@@ -550,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AWR45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,6 +665,14 @@
         <v>25</v>
       </c>
       <c r="C7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:1292" x14ac:dyDescent="0.3">
@@ -4511,7 +4527,10 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -7074,10 +7093,18 @@
     </row>
     <row r="16" spans="1:1292" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="3"/>
       <c r="L16" s="7"/>
       <c r="T16"/>
       <c r="U16"/>
@@ -10913,7 +10940,15 @@
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="3"/>
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:1292" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -13475,8 +13510,7 @@
       <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
       <c r="L22" s="7"/>
       <c r="T22"/>
       <c r="U22"/>

</xml_diff>